<commit_message>
update on 2-view system
4視点システムで構築したファイバー検出コードを2視点システムに移植

4視点システムの方ではplot_save_sxrの改良を開始
</commit_message>
<xml_diff>
--- a/Soft X-ray/Four-View/fiberPositions.xlsx
+++ b/Soft X-ray/Four-View/fiberPositions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shinjirotakeda/Documents/GitHub/test-open/Soft X-ray/Four-View/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8151C1-0BF5-8A43-9850-F59A8A2988D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E152C26D-4AD9-1E42-8814-B48CAD33651E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1100" windowWidth="28800" windowHeight="16160" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1100" windowWidth="28800" windowHeight="16160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="230921" sheetId="4" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="230721" sheetId="1" r:id="rId4"/>
     <sheet name="230712" sheetId="2" r:id="rId5"/>
     <sheet name="230920" sheetId="6" r:id="rId6"/>
-    <sheet name="240111_backup" sheetId="8" r:id="rId7"/>
-    <sheet name="240111" sheetId="7" r:id="rId8"/>
-    <sheet name="240501_old" sheetId="10" r:id="rId9"/>
-    <sheet name="240501_old2" sheetId="9" r:id="rId10"/>
-    <sheet name="240501" sheetId="11" r:id="rId11"/>
+    <sheet name="240111" sheetId="12" r:id="rId7"/>
+    <sheet name="240111_backup" sheetId="8" r:id="rId8"/>
+    <sheet name="240111_old" sheetId="7" r:id="rId9"/>
+    <sheet name="240501_old" sheetId="10" r:id="rId10"/>
+    <sheet name="240501_old2" sheetId="9" r:id="rId11"/>
+    <sheet name="240501" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="23">
   <si>
     <t>center_X</t>
     <phoneticPr fontId="1"/>
@@ -1737,6 +1738,586 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06735BCB-ED1E-904B-B816-90CA8290FBD5}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1618.8746535296575</v>
+      </c>
+      <c r="D2">
+        <v>996.0845244489575</v>
+      </c>
+      <c r="E2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1615.9734582162946</v>
+      </c>
+      <c r="D3">
+        <v>460</v>
+      </c>
+      <c r="E3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1246.9999999999998</v>
+      </c>
+      <c r="D4">
+        <v>457</v>
+      </c>
+      <c r="E4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1251.3493827116019</v>
+      </c>
+      <c r="D5">
+        <v>1002.3012493082249</v>
+      </c>
+      <c r="E5">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>879.52484896262547</v>
+      </c>
+      <c r="D6">
+        <v>1003.5206728589721</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>864.4076645902577</v>
+      </c>
+      <c r="D7">
+        <v>453.79481902986134</v>
+      </c>
+      <c r="E7">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>482.46508385439239</v>
+      </c>
+      <c r="D8">
+        <v>456.4455764172319</v>
+      </c>
+      <c r="E8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>496.99999999999994</v>
+      </c>
+      <c r="D9">
+        <v>996.09806950120878</v>
+      </c>
+      <c r="E9">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1630.7425030099457</v>
+      </c>
+      <c r="D10">
+        <v>851.02871194456884</v>
+      </c>
+      <c r="E10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1621.4061483041658</v>
+      </c>
+      <c r="D11">
+        <v>316.32671346786896</v>
+      </c>
+      <c r="E11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1255</v>
+      </c>
+      <c r="D12">
+        <v>311</v>
+      </c>
+      <c r="E12">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1262.520209029972</v>
+      </c>
+      <c r="D13">
+        <v>854.01460290365162</v>
+      </c>
+      <c r="E13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>890.62459762139895</v>
+      </c>
+      <c r="D14">
+        <v>854.04376388709545</v>
+      </c>
+      <c r="E14">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>874.28458590452396</v>
+      </c>
+      <c r="D15">
+        <v>308.24413555490423</v>
+      </c>
+      <c r="E15">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>495.83493585304365</v>
+      </c>
+      <c r="D16">
+        <v>307.79972769377798</v>
+      </c>
+      <c r="E16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>503.0101420458949</v>
+      </c>
+      <c r="D17">
+        <v>852</v>
+      </c>
+      <c r="E17">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1473</v>
+      </c>
+      <c r="D18">
+        <v>986</v>
+      </c>
+      <c r="E18">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1465.3355062255928</v>
+      </c>
+      <c r="D19">
+        <v>444.68324673024046</v>
+      </c>
+      <c r="E19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>1093</v>
+      </c>
+      <c r="D20">
+        <v>442.06282172105097</v>
+      </c>
+      <c r="E20">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1100.0510306101908</v>
+      </c>
+      <c r="D21">
+        <v>987.25802220168634</v>
+      </c>
+      <c r="E21">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>726.28422113454724</v>
+      </c>
+      <c r="D22">
+        <v>983.28024475973484</v>
+      </c>
+      <c r="E22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>708.43600904846016</v>
+      </c>
+      <c r="D23">
+        <v>441.80569376586431</v>
+      </c>
+      <c r="E23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>331.48909359995025</v>
+      </c>
+      <c r="D24">
+        <v>441.47228629221291</v>
+      </c>
+      <c r="E24">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>347.68442286943787</v>
+      </c>
+      <c r="D25">
+        <v>978.32923481001239</v>
+      </c>
+      <c r="E25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1480.3846762361873</v>
+      </c>
+      <c r="D26">
+        <v>845.182620379632</v>
+      </c>
+      <c r="E26">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1469.7054596333444</v>
+      </c>
+      <c r="D27">
+        <v>304.98346611431509</v>
+      </c>
+      <c r="E27">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>1097.5063568822814</v>
+      </c>
+      <c r="D28">
+        <v>304.46121207422669</v>
+      </c>
+      <c r="E28">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>1106.5494197876064</v>
+      </c>
+      <c r="D29">
+        <v>844</v>
+      </c>
+      <c r="E29">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>730.37055943669645</v>
+      </c>
+      <c r="D30">
+        <v>845.87694241073473</v>
+      </c>
+      <c r="E30">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>715</v>
+      </c>
+      <c r="D31">
+        <v>303</v>
+      </c>
+      <c r="E31">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>338.59998908096031</v>
+      </c>
+      <c r="D32">
+        <v>303.18836282597613</v>
+      </c>
+      <c r="E32">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>348.52787151824356</v>
+      </c>
+      <c r="D33">
+        <v>841.00000000000011</v>
+      </c>
+      <c r="E33">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -2318,11 +2899,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -6532,6 +7113,586 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="20"/>
+  <cols>
+    <col min="1" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1623.4265443435393</v>
+      </c>
+      <c r="D2">
+        <v>348.1904554392429</v>
+      </c>
+      <c r="E2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1625.5832371432114</v>
+      </c>
+      <c r="D3">
+        <v>883</v>
+      </c>
+      <c r="E3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1263.4976351483458</v>
+      </c>
+      <c r="D4">
+        <v>884.50371781189858</v>
+      </c>
+      <c r="E4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1255.2992618674946</v>
+      </c>
+      <c r="D5">
+        <v>339.8398448017395</v>
+      </c>
+      <c r="E5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>875.39997528745789</v>
+      </c>
+      <c r="D6">
+        <v>338.15420968300811</v>
+      </c>
+      <c r="E6">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>887.0054514726379</v>
+      </c>
+      <c r="D7">
+        <v>886.00067032311472</v>
+      </c>
+      <c r="E7">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>506.458800788433</v>
+      </c>
+      <c r="D8">
+        <v>879.01899490184496</v>
+      </c>
+      <c r="E8">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>495</v>
+      </c>
+      <c r="D9">
+        <v>338</v>
+      </c>
+      <c r="E9">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1614</v>
+      </c>
+      <c r="D10">
+        <v>493.5340062361679</v>
+      </c>
+      <c r="E10">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1618.4630275922909</v>
+      </c>
+      <c r="D11">
+        <v>1029.9493538404563</v>
+      </c>
+      <c r="E11">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>1249.6105560128537</v>
+      </c>
+      <c r="D12">
+        <v>1036.1994263586266</v>
+      </c>
+      <c r="E12">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1245.8986241372759</v>
+      </c>
+      <c r="D13">
+        <v>492.98930052173625</v>
+      </c>
+      <c r="E13">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>862.11815473245372</v>
+      </c>
+      <c r="D14">
+        <v>485.1151043261882</v>
+      </c>
+      <c r="E14">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>875.30901366636238</v>
+      </c>
+      <c r="D15">
+        <v>1032.3414742931636</v>
+      </c>
+      <c r="E15">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>493.06667877099005</v>
+      </c>
+      <c r="D16">
+        <v>1027.4941583555815</v>
+      </c>
+      <c r="E16">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>482.03760659484539</v>
+      </c>
+      <c r="D17">
+        <v>485.63522811947422</v>
+      </c>
+      <c r="E17">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1471</v>
+      </c>
+      <c r="D18">
+        <v>336</v>
+      </c>
+      <c r="E18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>1478.4170525137188</v>
+      </c>
+      <c r="D19">
+        <v>875.80732756498946</v>
+      </c>
+      <c r="E19">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>1105.8380913459309</v>
+      </c>
+      <c r="D20">
+        <v>875.36948917416635</v>
+      </c>
+      <c r="E20">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1097.9999999999998</v>
+      </c>
+      <c r="D21">
+        <v>330.46386067619034</v>
+      </c>
+      <c r="E21">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>717.66826419851839</v>
+      </c>
+      <c r="D22">
+        <v>328.37423485472425</v>
+      </c>
+      <c r="E22">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>729</v>
+      </c>
+      <c r="D23">
+        <v>872</v>
+      </c>
+      <c r="E23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>347.66064541799346</v>
+      </c>
+      <c r="D24">
+        <v>869.97155739522611</v>
+      </c>
+      <c r="E24">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>337.1778550489546</v>
+      </c>
+      <c r="D25">
+        <v>328.41781057527805</v>
+      </c>
+      <c r="E25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1463</v>
+      </c>
+      <c r="D26">
+        <v>476</v>
+      </c>
+      <c r="E26">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>1469.0269453062842</v>
+      </c>
+      <c r="D27">
+        <v>1016.9619501882065</v>
+      </c>
+      <c r="E27">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>1096.5015147541376</v>
+      </c>
+      <c r="D28">
+        <v>1019.4988351453728</v>
+      </c>
+      <c r="E28">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>1090</v>
+      </c>
+      <c r="D29">
+        <v>474</v>
+      </c>
+      <c r="E29">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>705.00866303979069</v>
+      </c>
+      <c r="D30">
+        <v>470.17576007912305</v>
+      </c>
+      <c r="E30">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31">
+        <v>720.70855122616899</v>
+      </c>
+      <c r="D31">
+        <v>1017.2579986889109</v>
+      </c>
+      <c r="E31">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>342.52202340700165</v>
+      </c>
+      <c r="D32">
+        <v>1008.9625696988209</v>
+      </c>
+      <c r="E32">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33">
+        <v>326.49685359317334</v>
+      </c>
+      <c r="D33">
+        <v>471.008965874051</v>
+      </c>
+      <c r="E33">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B4C6AA-75FF-D04D-AEB0-D50F87D3190D}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -7111,7 +8272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
@@ -7689,584 +8850,4 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06735BCB-ED1E-904B-B816-90CA8290FBD5}">
-  <dimension ref="A1:E33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="20"/>
-  <cols>
-    <col min="1" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1618.8746535296575</v>
-      </c>
-      <c r="D2">
-        <v>996.0845244489575</v>
-      </c>
-      <c r="E2">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1615.9734582162946</v>
-      </c>
-      <c r="D3">
-        <v>460</v>
-      </c>
-      <c r="E3">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1246.9999999999998</v>
-      </c>
-      <c r="D4">
-        <v>457</v>
-      </c>
-      <c r="E4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>1251.3493827116019</v>
-      </c>
-      <c r="D5">
-        <v>1002.3012493082249</v>
-      </c>
-      <c r="E5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>879.52484896262547</v>
-      </c>
-      <c r="D6">
-        <v>1003.5206728589721</v>
-      </c>
-      <c r="E6">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>864.4076645902577</v>
-      </c>
-      <c r="D7">
-        <v>453.79481902986134</v>
-      </c>
-      <c r="E7">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>482.46508385439239</v>
-      </c>
-      <c r="D8">
-        <v>456.4455764172319</v>
-      </c>
-      <c r="E8">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <v>496.99999999999994</v>
-      </c>
-      <c r="D9">
-        <v>996.09806950120878</v>
-      </c>
-      <c r="E9">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1630.7425030099457</v>
-      </c>
-      <c r="D10">
-        <v>851.02871194456884</v>
-      </c>
-      <c r="E10">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>1621.4061483041658</v>
-      </c>
-      <c r="D11">
-        <v>316.32671346786896</v>
-      </c>
-      <c r="E11">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>1255</v>
-      </c>
-      <c r="D12">
-        <v>311</v>
-      </c>
-      <c r="E12">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>1262.520209029972</v>
-      </c>
-      <c r="D13">
-        <v>854.01460290365162</v>
-      </c>
-      <c r="E13">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>890.62459762139895</v>
-      </c>
-      <c r="D14">
-        <v>854.04376388709545</v>
-      </c>
-      <c r="E14">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>874.28458590452396</v>
-      </c>
-      <c r="D15">
-        <v>308.24413555490423</v>
-      </c>
-      <c r="E15">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16">
-        <v>2</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>495.83493585304365</v>
-      </c>
-      <c r="D16">
-        <v>307.79972769377798</v>
-      </c>
-      <c r="E16">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>503.0101420458949</v>
-      </c>
-      <c r="D17">
-        <v>852</v>
-      </c>
-      <c r="E17">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18">
-        <v>3</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18">
-        <v>1473</v>
-      </c>
-      <c r="D18">
-        <v>986</v>
-      </c>
-      <c r="E18">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19">
-        <v>3</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>1465.3355062255928</v>
-      </c>
-      <c r="D19">
-        <v>444.68324673024046</v>
-      </c>
-      <c r="E19">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>1093</v>
-      </c>
-      <c r="D20">
-        <v>442.06282172105097</v>
-      </c>
-      <c r="E20">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>3</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>1100.0510306101908</v>
-      </c>
-      <c r="D21">
-        <v>987.25802220168634</v>
-      </c>
-      <c r="E21">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22">
-        <v>3</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-      <c r="C22">
-        <v>726.28422113454724</v>
-      </c>
-      <c r="D22">
-        <v>983.28024475973484</v>
-      </c>
-      <c r="E22">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23">
-        <v>3</v>
-      </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
-      <c r="C23">
-        <v>708.43600904846016</v>
-      </c>
-      <c r="D23">
-        <v>441.80569376586431</v>
-      </c>
-      <c r="E23">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24">
-        <v>331.48909359995025</v>
-      </c>
-      <c r="D24">
-        <v>441.47228629221291</v>
-      </c>
-      <c r="E24">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25">
-        <v>3</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-      <c r="C25">
-        <v>347.68442286943787</v>
-      </c>
-      <c r="D25">
-        <v>978.32923481001239</v>
-      </c>
-      <c r="E25">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>1480.3846762361873</v>
-      </c>
-      <c r="D26">
-        <v>845.182620379632</v>
-      </c>
-      <c r="E26">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>1469.7054596333444</v>
-      </c>
-      <c r="D27">
-        <v>304.98346611431509</v>
-      </c>
-      <c r="E27">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28">
-        <v>4</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>1097.5063568822814</v>
-      </c>
-      <c r="D28">
-        <v>304.46121207422669</v>
-      </c>
-      <c r="E28">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29">
-        <v>1106.5494197876064</v>
-      </c>
-      <c r="D29">
-        <v>844</v>
-      </c>
-      <c r="E29">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30">
-        <v>4</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30">
-        <v>730.37055943669645</v>
-      </c>
-      <c r="D30">
-        <v>845.87694241073473</v>
-      </c>
-      <c r="E30">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31">
-        <v>4</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>715</v>
-      </c>
-      <c r="D31">
-        <v>303</v>
-      </c>
-      <c r="E31">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32">
-        <v>4</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32">
-        <v>338.59998908096031</v>
-      </c>
-      <c r="D32">
-        <v>303.18836282597613</v>
-      </c>
-      <c r="E32">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33">
-        <v>4</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33">
-        <v>348.52787151824356</v>
-      </c>
-      <c r="D33">
-        <v>841.00000000000011</v>
-      </c>
-      <c r="E33">
-        <v>65</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>